<commit_message>
added new functionality :upload excel file after deleting the existing table(sheets) in the project if exist. create new API for fetch all the sheets without filtering
</commit_message>
<xml_diff>
--- a/backend/uploads/Accounts.xlsx
+++ b/backend/uploads/Accounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\R.Sanjay\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81186AE-DC07-4B63-A830-900B798154AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A28912-A470-4ED6-88E2-69B00108DCC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>project_id</t>
   </si>
@@ -119,13 +119,19 @@
   </si>
   <si>
     <t>2024-06-30</t>
+  </si>
+  <si>
+    <t>Dept32</t>
+  </si>
+  <si>
+    <t>Dept44</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -137,6 +143,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -486,13 +498,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -718,7 +733,36 @@
         <v>32</v>
       </c>
     </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>73</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>43433.43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>83</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>23553.35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>